<commit_message>
added range.table and extended xlwings.pro.reports to deal with Excel tables
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/DEV/xlwings-reports/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CB5944-0F3C-5B41-82A4-63A9BEA93DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D4515-5F44-214A-BEC1-BEC6AEE628CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Updated Text for update_links</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -189,6 +192,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5CAE5B2-A62D-6645-9698-85133E7B71B9}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{BC1DA8C7-0423-6647-B5B2-A1F3006B5F02}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E89D39BF-432E-BB46-8256-C4737F204971}" name="{{ df1 }}"/>
+    <tableColumn id="2" xr3:uid="{02B4C4D9-53F9-A745-BFED-42AF2B693038}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D221FAED-6F42-EB48-9E93-D890C0AE54C8}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -580,12 +594,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4493BA1E-DB84-DF47-A368-8AC6CB9929C1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed shape.text property and added support for template text in shapes in xlwings Reports
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D4515-5F44-214A-BEC1-BEC6AEE628CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B2104E-B248-5649-90C2-703FA9D9CB60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Table1">Sheet1!$A$1</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>{{mystring}}</t>
   </si>
 </sst>
 </file>
@@ -192,6 +196,379 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFE98E74-69A1-F342-922B-1A05FAF4D489}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="787400"/>
+          <a:ext cx="2933700" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> is no </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>template</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>. So the formatting should be left untouched.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FEE61E5-3B72-BC4A-9E8F-67907F77E8AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1790700" y="3073400"/>
+          <a:ext cx="1625600" cy="1625600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This shows {{mystring}}.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7D2AF8-999C-434C-8D67-188023E37549}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="800100"/>
+          <a:ext cx="2933700" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> shows {{mystring}}.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA57421-BE45-E146-8CF7-1C89E3720E65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4864100" y="2514600"/>
+          <a:ext cx="2933700" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>{{mystring}}</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB736D96-58D2-C24A-B16C-8B3C5875F651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1816100" y="5067300"/>
+          <a:ext cx="1625600" cy="1625600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4493BA1E-DB84-DF47-A368-8AC6CB9929C1}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -616,4 +993,25 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC216D76-32B9-9648-A341-8FA69A3F5929}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed markdown in reports
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B2104E-B248-5649-90C2-703FA9D9CB60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A83A55E-C14B-4A18-9AEF-49479A42ADA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="5" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Table1">Sheet1!$A$1</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -74,6 +75,9 @@
   </si>
   <si>
     <t>{{mystring}}</t>
+  </si>
+  <si>
+    <t>{{ markdown_cell }}</t>
   </si>
 </sst>
 </file>
@@ -571,6 +575,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64079561-051D-47B9-8DD9-581E22674897}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4143375" y="1281113"/>
+          <a:ext cx="5324475" cy="4019550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>{{ markdown_shape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> }}</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5CAE5B2-A62D-6645-9698-85133E7B71B9}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{BC1DA8C7-0423-6647-B5B2-A1F3006B5F02}"/>
@@ -886,12 +961,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -927,19 +1002,19 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -957,9 +1032,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -977,9 +1052,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -999,15 +1074,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC216D76-32B9-9648-A341-8FA69A3F5929}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5458166E-239E-40A5-8BB1-75BE41AF2DB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Font, Characters and Markdown support (#1536)
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B2104E-B248-5649-90C2-703FA9D9CB60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A83A55E-C14B-4A18-9AEF-49479A42ADA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3860" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="5" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Table1">Sheet1!$A$1</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -74,6 +75,9 @@
   </si>
   <si>
     <t>{{mystring}}</t>
+  </si>
+  <si>
+    <t>{{ markdown_cell }}</t>
   </si>
 </sst>
 </file>
@@ -571,6 +575,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64079561-051D-47B9-8DD9-581E22674897}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4143375" y="1281113"/>
+          <a:ext cx="5324475" cy="4019550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>{{ markdown_shape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> }}</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5CAE5B2-A62D-6645-9698-85133E7B71B9}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{BC1DA8C7-0423-6647-B5B2-A1F3006B5F02}"/>
@@ -886,12 +961,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -927,19 +1002,19 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -957,9 +1032,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -977,9 +1052,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -999,15 +1074,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC216D76-32B9-9648-A341-8FA69A3F5929}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5458166E-239E-40A5-8BB1-75BE41AF2DB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added aggsmall df filter
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C48368-E0CC-8D43-9760-EEECF3F223EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF92C13E-69E7-B84E-B68D-B462011E117A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="7" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>{{ pic | scale(1.2) }}</t>
+  </si>
+  <si>
+    <t>{{ df | aggsmall(1, 3) }}</t>
+  </si>
+  <si>
+    <t>{{ df }}</t>
+  </si>
+  <si>
+    <t>{{ df | aggsmall(8, 3) }}</t>
+  </si>
+  <si>
+    <t>{{ df | aggsmall(5, 3) }}</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1056,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -1201,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2149,6 +2161,351 @@
         <v>7</v>
       </c>
       <c r="K76" s="2"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>38</v>
+      </c>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G80" s="2">
+        <v>0</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="2">
+        <v>4</v>
+      </c>
+      <c r="J80" s="2">
+        <v>1</v>
+      </c>
+      <c r="K80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G81" s="2">
+        <v>1</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I81" s="2">
+        <v>2</v>
+      </c>
+      <c r="J81" s="2">
+        <v>2</v>
+      </c>
+      <c r="K81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G82" s="2">
+        <v>2</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I82" s="2">
+        <v>6</v>
+      </c>
+      <c r="J82" s="2">
+        <v>5</v>
+      </c>
+      <c r="K82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G83" s="2">
+        <v>3</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I83" s="2">
+        <v>6</v>
+      </c>
+      <c r="J83" s="2">
+        <v>7</v>
+      </c>
+      <c r="K83" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G84" s="2">
+        <v>4</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I84" s="2">
+        <v>9</v>
+      </c>
+      <c r="J84" s="2">
+        <v>8</v>
+      </c>
+      <c r="K84" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>39</v>
+      </c>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G87" s="2">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I87" s="2">
+        <v>4</v>
+      </c>
+      <c r="J87" s="2">
+        <v>1</v>
+      </c>
+      <c r="K87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G88" s="2">
+        <v>1</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I88" s="2">
+        <v>2</v>
+      </c>
+      <c r="J88" s="2">
+        <v>2</v>
+      </c>
+      <c r="K88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G89" s="2">
+        <v>2</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I89" s="2">
+        <v>6</v>
+      </c>
+      <c r="J89" s="2">
+        <v>5</v>
+      </c>
+      <c r="K89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G90" s="2">
+        <v>3</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I90" s="2">
+        <v>6</v>
+      </c>
+      <c r="J90" s="2">
+        <v>7</v>
+      </c>
+      <c r="K90" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G91" s="2">
+        <v>4</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I91" s="2">
+        <v>9</v>
+      </c>
+      <c r="J91" s="2">
+        <v>8</v>
+      </c>
+      <c r="K91" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>40</v>
+      </c>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G94" s="2">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I94" s="2">
+        <v>27</v>
+      </c>
+      <c r="J94" s="2">
+        <v>23</v>
+      </c>
+      <c r="K94" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>41</v>
+      </c>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G97" s="2">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I97" s="2">
+        <v>6</v>
+      </c>
+      <c r="J97" s="2">
+        <v>7</v>
+      </c>
+      <c r="K97" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G98" s="2">
+        <v>1</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I98" s="2">
+        <v>9</v>
+      </c>
+      <c r="J98" s="2">
+        <v>8</v>
+      </c>
+      <c r="K98" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G99" s="2">
+        <v>2</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I99" s="2">
+        <v>12</v>
+      </c>
+      <c r="J99" s="2">
+        <v>8</v>
+      </c>
+      <c r="K99" s="2">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2159,7 +2516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32FA9A8-60DD-344B-BC1D-0DAA1906625F}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added "body" filter for dataframes
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D609218D-C331-4665-8E53-66C7C93F0DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0581154F-0A41-44C0-98AE-F1AB855C3CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>{{ df | aggsmall(5, 3, Other, 0) }}</t>
+  </si>
+  <si>
+    <t>{{ df | body }}</t>
   </si>
 </sst>
 </file>
@@ -1213,9 +1216,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J105" sqref="J105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -2454,7 +2459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="7:11" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G97" s="2">
         <v>0</v>
       </c>
@@ -2471,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="7:11" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G98" s="2">
         <v>1</v>
       </c>
@@ -2488,7 +2493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="7:11" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G99" s="2">
         <v>2</v>
       </c>
@@ -2505,8 +2510,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A101" t="s">
+        <v>42</v>
+      </c>
+      <c r="G101" s="2">
+        <v>1</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G102" s="2">
+        <v>1</v>
+      </c>
+      <c r="H102" s="2">
+        <v>1</v>
+      </c>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added DatFrame reports filters head and tail, closes #1633
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0581154F-0A41-44C0-98AE-F1AB855C3CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9F813-6C36-8E4A-8513-8BC07575E451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -151,9 +151,6 @@
     <t>{{ pic | scale(1.2) }}</t>
   </si>
   <si>
-    <t>{{ df }}</t>
-  </si>
-  <si>
     <t>{{ df2 | noindex | maxrows(3, Other, 0) }}</t>
   </si>
   <si>
@@ -163,16 +160,22 @@
     <t>{{ df2 | noindex | maxrows(10, Other) }}</t>
   </si>
   <si>
-    <t>{{ df | aggsmall(1, 3, Other) }}</t>
-  </si>
-  <si>
-    <t>{{ df | aggsmall(8, 3, Other, 0) }}</t>
-  </si>
-  <si>
-    <t>{{ df | aggsmall(5, 3, Other, 0) }}</t>
-  </si>
-  <si>
-    <t>{{ df | body }}</t>
+    <t>{{ df2 | aggsmall(1, 3, Other) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | aggsmall(8, 3, Other, 0) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | head(3) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | tail(2) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | body }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | aggsmall(5, 3, Other) }}</t>
   </si>
 </sst>
 </file>
@@ -1063,12 +1066,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1104,19 +1107,19 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1134,9 +1137,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1154,9 +1157,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1180,9 +1183,9 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1201,9 +1204,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1216,15 +1219,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J105" sqref="J105"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1241,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1251,7 +1254,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1264,14 +1267,14 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="2">
         <v>1</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" s="2">
         <v>1</v>
       </c>
@@ -1307,21 +1310,21 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1337,7 +1340,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1350,28 +1353,28 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1385,7 +1388,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G16" s="2">
         <v>1</v>
       </c>
@@ -1396,28 +1399,28 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1457,21 +1460,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G26" s="2">
         <v>1</v>
       </c>
@@ -1496,7 +1499,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G27" s="2">
         <v>1</v>
       </c>
@@ -1507,21 +1510,21 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1535,7 +1538,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G31" s="2">
         <v>1</v>
       </c>
@@ -1546,28 +1549,28 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G36" s="2">
         <v>0</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G37" s="2">
         <v>1</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G38" s="2">
         <v>2</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G39" s="2">
         <v>3</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G40" s="2">
         <v>4</v>
       </c>
@@ -1670,23 +1673,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>25</v>
@@ -1702,7 +1705,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G44" s="2" t="s">
         <v>29</v>
       </c>
@@ -1717,7 +1720,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G45" s="2" t="s">
         <v>26</v>
       </c>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G46" s="2" t="s">
         <v>31</v>
       </c>
@@ -1747,21 +1750,21 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G50" s="2">
         <v>1</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G51" s="2">
         <v>0</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G52" s="2">
         <v>2</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G53" s="2">
         <v>3</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G54" s="2">
         <v>4</v>
       </c>
@@ -1864,21 +1867,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G58" s="2">
         <v>4</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="2">
         <v>3</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G60" s="2">
         <v>2</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G61" s="2">
         <v>0</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G62" s="2">
         <v>1</v>
       </c>
@@ -1981,23 +1984,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>25</v>
@@ -2013,7 +2016,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G66" s="2" t="s">
         <v>26</v>
       </c>
@@ -2028,7 +2031,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G67" s="2" t="s">
         <v>29</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G68" s="2" t="s">
         <v>31</v>
       </c>
@@ -2058,23 +2061,23 @@
       </c>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>25</v>
@@ -2090,7 +2093,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G72" s="2" t="s">
         <v>29</v>
       </c>
@@ -2105,7 +2108,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G73" s="2" t="s">
         <v>26</v>
       </c>
@@ -2120,7 +2123,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G74" s="2" t="s">
         <v>27</v>
       </c>
@@ -2135,7 +2138,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G75" s="2" t="s">
         <v>28</v>
       </c>
@@ -2150,7 +2153,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G76" s="2" t="s">
         <v>30</v>
       </c>
@@ -2165,23 +2168,23 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2" t="s">
@@ -2197,7 +2200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G80" s="2">
         <v>0</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G81" s="2">
         <v>1</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G82" s="2">
         <v>2</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G83" s="2">
         <v>3</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G84" s="2">
         <v>4</v>
       </c>
@@ -2282,16 +2285,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2" t="s">
@@ -2307,7 +2310,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G87" s="2">
         <v>0</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G88" s="2">
         <v>1</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G89" s="2">
         <v>2</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G90" s="2">
         <v>3</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G91" s="2">
         <v>4</v>
       </c>
@@ -2392,16 +2395,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2" t="s">
@@ -2417,9 +2420,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G94" s="2">
-        <v>0</v>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G94" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>31</v>
@@ -2434,16 +2437,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2" t="s">
@@ -2459,9 +2462,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G97" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>28</v>
@@ -2476,9 +2479,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G98" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>30</v>
@@ -2493,13 +2496,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G99" s="2">
-        <v>2</v>
-      </c>
-      <c r="H99" s="2" t="s">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G99" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H99" s="2"/>
       <c r="I99" s="2">
         <v>12</v>
       </c>
@@ -2510,14 +2511,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -2531,7 +2532,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G102" s="2">
         <v>1</v>
       </c>
@@ -2541,6 +2542,162 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>40</v>
+      </c>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I105" s="2">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2">
+        <v>1</v>
+      </c>
+      <c r="K105" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G106" s="2">
+        <v>1</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I106" s="2">
+        <v>2</v>
+      </c>
+      <c r="J106" s="2">
+        <v>2</v>
+      </c>
+      <c r="K106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G107" s="2">
+        <v>2</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I107" s="2">
+        <v>6</v>
+      </c>
+      <c r="J107" s="2">
+        <v>5</v>
+      </c>
+      <c r="K107" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>41</v>
+      </c>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G113" s="2">
+        <v>3</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113" s="2">
+        <v>6</v>
+      </c>
+      <c r="J113" s="2">
+        <v>7</v>
+      </c>
+      <c r="K113" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G114" s="2">
+        <v>4</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I114" s="2">
+        <v>9</v>
+      </c>
+      <c r="J114" s="2">
+        <v>8</v>
+      </c>
+      <c r="K114" s="2">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2556,24 +2713,24 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
added DatFrame reports filters head and tail, closes #1633 (#1636)
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0581154F-0A41-44C0-98AE-F1AB855C3CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9F813-6C36-8E4A-8513-8BC07575E451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -151,9 +151,6 @@
     <t>{{ pic | scale(1.2) }}</t>
   </si>
   <si>
-    <t>{{ df }}</t>
-  </si>
-  <si>
     <t>{{ df2 | noindex | maxrows(3, Other, 0) }}</t>
   </si>
   <si>
@@ -163,16 +160,22 @@
     <t>{{ df2 | noindex | maxrows(10, Other) }}</t>
   </si>
   <si>
-    <t>{{ df | aggsmall(1, 3, Other) }}</t>
-  </si>
-  <si>
-    <t>{{ df | aggsmall(8, 3, Other, 0) }}</t>
-  </si>
-  <si>
-    <t>{{ df | aggsmall(5, 3, Other, 0) }}</t>
-  </si>
-  <si>
-    <t>{{ df | body }}</t>
+    <t>{{ df2 | aggsmall(1, 3, Other) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | aggsmall(8, 3, Other, 0) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | head(3) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | tail(2) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | body }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | aggsmall(5, 3, Other) }}</t>
   </si>
 </sst>
 </file>
@@ -1063,12 +1066,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.8125" style="1"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1104,19 +1107,19 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1134,9 +1137,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1154,9 +1157,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1180,9 +1183,9 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1201,9 +1204,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1216,15 +1219,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J105" sqref="J105"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1241,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1251,7 +1254,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1264,14 +1267,14 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="2">
         <v>1</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" s="2">
         <v>1</v>
       </c>
@@ -1307,21 +1310,21 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1337,7 +1340,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1350,28 +1353,28 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1385,7 +1388,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G16" s="2">
         <v>1</v>
       </c>
@@ -1396,28 +1399,28 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1457,21 +1460,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G26" s="2">
         <v>1</v>
       </c>
@@ -1496,7 +1499,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G27" s="2">
         <v>1</v>
       </c>
@@ -1507,21 +1510,21 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1535,7 +1538,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G31" s="2">
         <v>1</v>
       </c>
@@ -1546,28 +1549,28 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G36" s="2">
         <v>0</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G37" s="2">
         <v>1</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G38" s="2">
         <v>2</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G39" s="2">
         <v>3</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G40" s="2">
         <v>4</v>
       </c>
@@ -1670,23 +1673,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>25</v>
@@ -1702,7 +1705,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G44" s="2" t="s">
         <v>29</v>
       </c>
@@ -1717,7 +1720,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G45" s="2" t="s">
         <v>26</v>
       </c>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G46" s="2" t="s">
         <v>31</v>
       </c>
@@ -1747,21 +1750,21 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G50" s="2">
         <v>1</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G51" s="2">
         <v>0</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G52" s="2">
         <v>2</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G53" s="2">
         <v>3</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G54" s="2">
         <v>4</v>
       </c>
@@ -1864,21 +1867,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G58" s="2">
         <v>4</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="2">
         <v>3</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G60" s="2">
         <v>2</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G61" s="2">
         <v>0</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G62" s="2">
         <v>1</v>
       </c>
@@ -1981,23 +1984,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>25</v>
@@ -2013,7 +2016,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G66" s="2" t="s">
         <v>26</v>
       </c>
@@ -2028,7 +2031,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G67" s="2" t="s">
         <v>29</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G68" s="2" t="s">
         <v>31</v>
       </c>
@@ -2058,23 +2061,23 @@
       </c>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>25</v>
@@ -2090,7 +2093,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G72" s="2" t="s">
         <v>29</v>
       </c>
@@ -2105,7 +2108,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G73" s="2" t="s">
         <v>26</v>
       </c>
@@ -2120,7 +2123,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G74" s="2" t="s">
         <v>27</v>
       </c>
@@ -2135,7 +2138,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G75" s="2" t="s">
         <v>28</v>
       </c>
@@ -2150,7 +2153,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G76" s="2" t="s">
         <v>30</v>
       </c>
@@ -2165,23 +2168,23 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2" t="s">
@@ -2197,7 +2200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G80" s="2">
         <v>0</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G81" s="2">
         <v>1</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G82" s="2">
         <v>2</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G83" s="2">
         <v>3</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G84" s="2">
         <v>4</v>
       </c>
@@ -2282,16 +2285,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2" t="s">
@@ -2307,7 +2310,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G87" s="2">
         <v>0</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G88" s="2">
         <v>1</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G89" s="2">
         <v>2</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G90" s="2">
         <v>3</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G91" s="2">
         <v>4</v>
       </c>
@@ -2392,16 +2395,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2" t="s">
@@ -2417,9 +2420,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G94" s="2">
-        <v>0</v>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G94" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>31</v>
@@ -2434,16 +2437,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2" t="s">
@@ -2459,9 +2462,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G97" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>28</v>
@@ -2476,9 +2479,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G98" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>30</v>
@@ -2493,13 +2496,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G99" s="2">
-        <v>2</v>
-      </c>
-      <c r="H99" s="2" t="s">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G99" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H99" s="2"/>
       <c r="I99" s="2">
         <v>12</v>
       </c>
@@ -2510,14 +2511,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -2531,7 +2532,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G102" s="2">
         <v>1</v>
       </c>
@@ -2541,6 +2542,162 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>40</v>
+      </c>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I105" s="2">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2">
+        <v>1</v>
+      </c>
+      <c r="K105" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G106" s="2">
+        <v>1</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I106" s="2">
+        <v>2</v>
+      </c>
+      <c r="J106" s="2">
+        <v>2</v>
+      </c>
+      <c r="K106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G107" s="2">
+        <v>2</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I107" s="2">
+        <v>6</v>
+      </c>
+      <c r="J107" s="2">
+        <v>5</v>
+      </c>
+      <c r="K107" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>41</v>
+      </c>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G113" s="2">
+        <v>3</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113" s="2">
+        <v>6</v>
+      </c>
+      <c r="J113" s="2">
+        <v>7</v>
+      </c>
+      <c r="K113" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G114" s="2">
+        <v>4</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I114" s="2">
+        <v>9</v>
+      </c>
+      <c r="J114" s="2">
+        <v>8</v>
+      </c>
+      <c r="K114" s="2">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2556,24 +2713,24 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
added colslice and rowslice filters
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9F813-6C36-8E4A-8513-8BC07575E451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319A1B23-E594-A54A-B2C4-81BD3294AAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="48">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>{{ df2 | aggsmall(5, 3, Other) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | rowslice(0, 3) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | colslice(3) | rowslice(0, 2) }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1219,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1428,8 +1440,12 @@
       <c r="H20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="K20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1481,7 +1497,9 @@
       <c r="G25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2665,7 +2683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G113" s="2">
         <v>3</v>
       </c>
@@ -2682,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G114" s="2">
         <v>4</v>
       </c>
@@ -2698,6 +2716,130 @@
       <c r="K114" s="2">
         <v>7</v>
       </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>44</v>
+      </c>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G117" s="2">
+        <v>0</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I117" s="2">
+        <v>4</v>
+      </c>
+      <c r="J117" s="2">
+        <v>1</v>
+      </c>
+      <c r="K117" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G118" s="2">
+        <v>1</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I118" s="2">
+        <v>2</v>
+      </c>
+      <c r="J118" s="2">
+        <v>2</v>
+      </c>
+      <c r="K118" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G119" s="2">
+        <v>2</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="2">
+        <v>6</v>
+      </c>
+      <c r="J119" s="2">
+        <v>5</v>
+      </c>
+      <c r="K119" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>45</v>
+      </c>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
+      <c r="H123" s="2">
+        <v>1</v>
+      </c>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G124" s="2">
+        <v>1</v>
+      </c>
+      <c r="H124" s="2">
+        <v>1</v>
+      </c>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added colslice and rowslice filters (#1645)
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9F813-6C36-8E4A-8513-8BC07575E451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319A1B23-E594-A54A-B2C4-81BD3294AAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="48">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>{{ df2 | aggsmall(5, 3, Other) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | rowslice(0, 3) }}</t>
+  </si>
+  <si>
+    <t>{{ df2 | colslice(3) | rowslice(0, 2) }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1219,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1428,8 +1440,12 @@
       <c r="H20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="K20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1481,7 +1497,9 @@
       <c r="G25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2665,7 +2683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G113" s="2">
         <v>3</v>
       </c>
@@ -2682,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G114" s="2">
         <v>4</v>
       </c>
@@ -2698,6 +2716,130 @@
       <c r="K114" s="2">
         <v>7</v>
       </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>44</v>
+      </c>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G117" s="2">
+        <v>0</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I117" s="2">
+        <v>4</v>
+      </c>
+      <c r="J117" s="2">
+        <v>1</v>
+      </c>
+      <c r="K117" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G118" s="2">
+        <v>1</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I118" s="2">
+        <v>2</v>
+      </c>
+      <c r="J118" s="2">
+        <v>2</v>
+      </c>
+      <c r="K118" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G119" s="2">
+        <v>2</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="2">
+        <v>6</v>
+      </c>
+      <c r="J119" s="2">
+        <v>5</v>
+      </c>
+      <c r="K119" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>45</v>
+      </c>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
+      <c r="H123" s="2">
+        <v>1</v>
+      </c>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G124" s="2">
+        <v>1</v>
+      </c>
+      <c r="H124" s="2">
+        <v>1</v>
+      </c>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added multiply/divide/subtract/add df filters
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7A4CF3-1A98-8745-B7F4-2F5D48FD9D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D070E867-9FAE-9F40-AD5E-9F3BAEFB24DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3980" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="60">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>Some text with a date: 12/13/10</t>
+  </si>
+  <si>
+    <t>{{ df1 | multiply(0, 100) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | divide(0, 100) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | add(1, 100) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | subtract(1, 100) }}</t>
   </si>
 </sst>
 </file>
@@ -1265,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
-  <dimension ref="A1:K124"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2874,6 +2886,194 @@
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>56</v>
+      </c>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G127" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H127" s="2">
+        <v>100</v>
+      </c>
+      <c r="I127" s="2">
+        <v>1</v>
+      </c>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G128" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H128" s="2">
+        <v>100</v>
+      </c>
+      <c r="I128" s="2">
+        <v>1</v>
+      </c>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>57</v>
+      </c>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G131" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H131" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I131" s="2">
+        <v>1</v>
+      </c>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G132" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H132" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I132" s="2">
+        <v>1</v>
+      </c>
+      <c r="J132" s="2"/>
+      <c r="K132" s="2"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2"/>
+      <c r="K133" s="2"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>58</v>
+      </c>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I134" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G135" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H135" s="2">
+        <v>1</v>
+      </c>
+      <c r="I135" s="2">
+        <v>101</v>
+      </c>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G136" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H136" s="2">
+        <v>1</v>
+      </c>
+      <c r="I136" s="2">
+        <v>101</v>
+      </c>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>59</v>
+      </c>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I138" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J138" s="2"/>
+      <c r="K138" s="2"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G139" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H139" s="2">
+        <v>1</v>
+      </c>
+      <c r="I139" s="2">
+        <v>-99</v>
+      </c>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G140" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H140" s="2">
+        <v>1</v>
+      </c>
+      <c r="I140" s="2">
+        <v>-99</v>
+      </c>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2925,7 +3125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244878F1-91C5-5849-8422-5F764409BB6B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
datetime fixes in reports package
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EC9360-0EDC-1C42-805C-894C5CF4B231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EDF195-D6C5-6141-BD4C-9D0EBB841EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
@@ -203,15 +203,6 @@
     <t>{{ mydate | datetime("%Y--%m--%d") }}</t>
   </si>
   <si>
-    <t>2010-12-13 00:00:00</t>
-  </si>
-  <si>
-    <t>2010--12--13</t>
-  </si>
-  <si>
-    <t>Some text with a date: 12/13/10</t>
-  </si>
-  <si>
     <t>{{ df1 | multiply(0, 100) }}</t>
   </si>
   <si>
@@ -227,7 +218,16 @@
     <t>Some text with a date: {{ mydate | datetime("%m/%d/%y") }}</t>
   </si>
   <si>
-    <t>December 13, 2010</t>
+    <t>2010-12-01 00:00:00</t>
+  </si>
+  <si>
+    <t>December 1, 2010</t>
+  </si>
+  <si>
+    <t>2010--12--01</t>
+  </si>
+  <si>
+    <t>Some text with a date: 12/01/10</t>
   </si>
 </sst>
 </file>
@@ -812,6 +812,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B73D8372-32F7-6F4F-A62D-A9A73412279B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="3022600"/>
+          <a:ext cx="3683000" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>{{ mydate | datetime }}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5CAE5B2-A62D-6645-9698-85133E7B71B9}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{BC1DA8C7-0423-6647-B5B2-A1F3006B5F02}"/>
@@ -2899,7 +2965,7 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2" t="s">
@@ -2946,7 +3012,7 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G130" s="2"/>
       <c r="H130" s="2" t="s">
@@ -2993,7 +3059,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G134" s="2"/>
       <c r="H134" s="2" t="s">
@@ -3040,7 +3106,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="2" t="s">
@@ -3129,7 +3195,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3142,7 +3208,7 @@
         <v>49</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -3157,7 +3223,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -3172,7 +3238,7 @@
         <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -3184,15 +3250,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added docs and tests for fontcolor filter
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3919518E-A03D-DA43-9DAB-08298753A480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3B657C-480F-8C41-91AC-D1B019A30E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="19200" windowHeight="21100" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>{{ df2 | sortasc(1) | maxrows(3, "Other", 1) | colslice(1) }}</t>
+  </si>
+  <si>
+    <t>{{ mystring | fontcolor("white") }}</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1184,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C37306-6492-634D-B59F-CECAA69C603C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1192,7 +1195,7 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,8 +1211,11 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1340,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reports: fontcolor filter (#1692)
* reports: added fontcolor filter
* allow to use black/white as name in the fontcolor filter
* added docs and tests for fontcolor filter
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3919518E-A03D-DA43-9DAB-08298753A480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3B657C-480F-8C41-91AC-D1B019A30E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="19200" windowHeight="21100" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
   <si>
     <t>{{ mystring }}</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>{{ df2 | sortasc(1) | maxrows(3, "Other", 1) | colslice(1) }}</t>
+  </si>
+  <si>
+    <t>{{ mystring | fontcolor("white") }}</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1184,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C37306-6492-634D-B59F-CECAA69C603C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1192,7 +1195,7 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,8 +1211,11 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1340,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reports (breaking change): aligned the args order in the arithmetics filters with all the other filters
</commit_message>
<xml_diff>
--- a/tests/reports/template1.xlsx
+++ b/tests/reports/template1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings\tests\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3B657C-480F-8C41-91AC-D1B019A30E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E530B-E3D2-4FD0-9F7E-337EE0823EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="6" xr2:uid="{6E9D0488-361A-C945-B3B9-0C9A6A0FFD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="Table1">Sheet1!$A$1</definedName>
     <definedName name="Table2">Sheet1!$A$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,18 +191,6 @@
     <t>{{ df2 | maxrows(10, "Other") | colslice(1) }}</t>
   </si>
   <si>
-    <t>{{ df1 | mul(1, 100) }}</t>
-  </si>
-  <si>
-    <t>{{ df1 | div(1, 100) }}</t>
-  </si>
-  <si>
-    <t>{{ df1 | add(2, 100) }}</t>
-  </si>
-  <si>
-    <t>{{ df1 | sub(2, 100) }}</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -225,6 +213,18 @@
   </si>
   <si>
     <t>{{ mystring | fontcolor("white") }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | mul(100, 1) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | div(100, 1) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | add(100, 2) }}</t>
+  </si>
+  <si>
+    <t>{{ df1 | sub(100, 2) }}</t>
   </si>
 </sst>
 </file>
@@ -1186,16 +1186,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,10 +1212,10 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1232,19 +1232,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1262,9 +1262,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1282,9 +1282,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1308,9 +1308,9 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1329,9 +1329,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1346,18 +1346,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130DEA-25D6-5E40-BFD3-A1E4C886A4E9}">
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1368,7 +1368,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1394,49 +1394,49 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1465,65 +1465,65 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>13</v>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G21" s="2">
         <v>1</v>
       </c>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G22" s="2">
         <v>1</v>
       </c>
@@ -1561,23 +1561,23 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>13</v>
@@ -1591,7 +1591,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G26" s="2">
         <v>1</v>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G27" s="2">
         <v>1</v>
       </c>
@@ -1613,23 +1613,23 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G30" s="2">
         <v>1</v>
@@ -1641,7 +1641,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G31" s="2">
         <v>1</v>
       </c>
@@ -1652,33 +1652,33 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>17</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>20</v>
@@ -1693,7 +1693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G36" s="2">
         <v>0</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G37" s="2">
         <v>1</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G38" s="2">
         <v>2</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G39" s="2">
         <v>3</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G40" s="2">
         <v>4</v>
       </c>
@@ -1778,23 +1778,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>20</v>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G44" s="2" t="s">
         <v>24</v>
       </c>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G45" s="2" t="s">
         <v>21</v>
       </c>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G46" s="2" t="s">
         <v>26</v>
       </c>
@@ -1855,26 +1855,26 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>18</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>20</v>
@@ -1889,7 +1889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G50" s="2">
         <v>0</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G51" s="2">
         <v>1</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G52" s="2">
         <v>2</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G53" s="2">
         <v>3</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G54" s="2">
         <v>4</v>
       </c>
@@ -1974,26 +1974,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>19</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>20</v>
@@ -2008,7 +2008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G58" s="2">
         <v>4</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G59" s="2">
         <v>3</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G60" s="2">
         <v>2</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G61" s="2">
         <v>1</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G62" s="2">
         <v>0</v>
       </c>
@@ -2093,23 +2093,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>20</v>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G66" s="2" t="s">
         <v>24</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G67" s="2" t="s">
         <v>21</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G68" s="2" t="s">
         <v>26</v>
       </c>
@@ -2170,21 +2170,21 @@
       </c>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G72" s="2" t="s">
         <v>24</v>
       </c>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G73" s="2" t="s">
         <v>21</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G74" s="2" t="s">
         <v>22</v>
       </c>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G75" s="2" t="s">
         <v>23</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G76" s="2" t="s">
         <v>25</v>
       </c>
@@ -2277,26 +2277,26 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
         <v>36</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>20</v>
@@ -2311,7 +2311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G80" s="2">
         <v>0</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G81" s="2">
         <v>1</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G82" s="2">
         <v>2</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G83" s="2">
         <v>3</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G84" s="2">
         <v>4</v>
       </c>
@@ -2396,19 +2396,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
         <v>17</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>20</v>
@@ -2423,7 +2423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G87" s="2">
         <v>0</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G88" s="2">
         <v>1</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G89" s="2">
         <v>2</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G90" s="2">
         <v>3</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G91" s="2">
         <v>4</v>
       </c>
@@ -2508,19 +2508,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>20</v>
@@ -2535,7 +2535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G94" s="2" t="s">
         <v>26</v>
       </c>
@@ -2550,75 +2550,75 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
         <v>30</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>20</v>
@@ -2633,7 +2633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G105" s="2">
         <v>0</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G106" s="2">
         <v>1</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G107" s="2">
         <v>2</v>
       </c>
@@ -2684,40 +2684,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A112" t="s">
         <v>31</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>20</v>
@@ -2732,7 +2732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G113" s="2">
         <v>3</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G114" s="2">
         <v>4</v>
       </c>
@@ -2766,19 +2766,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A116" t="s">
         <v>32</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>20</v>
@@ -2793,7 +2793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G117" s="2">
         <v>0</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G118" s="2">
         <v>1</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G119" s="2">
         <v>2</v>
       </c>
@@ -2844,21 +2844,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
         <v>33</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G123" s="2">
         <v>1</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G124" s="2">
         <v>2</v>
       </c>
@@ -2894,19 +2894,19 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
+        <v>56</v>
+      </c>
+      <c r="G126" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G126" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>13</v>
@@ -2917,7 +2917,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G127" s="2" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +2930,7 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G128" s="2" t="s">
         <v>16</v>
       </c>
@@ -2943,19 +2943,19 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>13</v>
@@ -2966,7 +2966,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G131" s="2" t="s">
         <v>15</v>
       </c>
@@ -2979,7 +2979,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G132" s="2" t="s">
         <v>16</v>
       </c>
@@ -2992,19 +2992,19 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>13</v>
@@ -3015,7 +3015,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G135" s="2" t="s">
         <v>15</v>
       </c>
@@ -3028,7 +3028,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G136" s="2" t="s">
         <v>16</v>
       </c>
@@ -3041,19 +3041,19 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>13</v>
@@ -3064,7 +3064,7 @@
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G139" s="2" t="s">
         <v>15</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.5">
       <c r="G140" s="2" t="s">
         <v>16</v>
       </c>
@@ -3104,34 +3104,34 @@
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3149,12 +3149,12 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.6875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -3164,12 +3164,12 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -3179,12 +3179,12 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
@@ -3194,12 +3194,12 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>

</xml_diff>